<commit_message>
Dergi submit edildi. Hayırlı olsun :) @ozank, @furkankarakaya
</commit_message>
<xml_diff>
--- a/Prototype/Test/test diaries/2019.05.13/13.05.2019_kalorimetre.xlsx
+++ b/Prototype/Test/test diaries/2019.05.13/13.05.2019_kalorimetre.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ugurm\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mesutto\Desktop\github work\IMMD\Prototype\Test\test diaries\2019.05.13\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -120,7 +120,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -474,7 +474,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -488,7 +488,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -771,6 +770,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D23D-41F5-A6D1-06CC452FFDDF}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -905,6 +909,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-D23D-41F5-A6D1-06CC452FFDDF}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1059,6 +1068,11 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000002-D23D-41F5-A6D1-06CC452FFDDF}"/>
+                  </c:ext>
+                </c:extLst>
               </c15:ser>
             </c15:filteredLineSeries>
           </c:ext>
@@ -2074,8 +2088,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G57" sqref="G57"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N49" sqref="N48:N49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>